<commit_message>
updating team meeting notes
</commit_message>
<xml_diff>
--- a/team_notes.xlsx
+++ b/team_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Información\GoDr gmail\DS4A\ds4a_team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1115F65-A97C-4710-8C8A-8AD154B46C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD092995-3F5B-431F-853B-E2FB4F68D1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{5DAA10E0-1AEE-4ECB-B698-597DDCB68611}"/>
   </bookViews>
@@ -509,64 +509,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76F95E4-9CC0-4B4E-8E01-4589602999B0}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.42578125" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.7109375" customWidth="1"/>
+    <col min="4" max="4" width="68.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -574,7 +562,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -582,7 +570,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -590,7 +578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -598,7 +586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -606,7 +594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -614,7 +602,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -622,7 +610,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -630,7 +618,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -644,6 +632,26 @@
       </c>
       <c r="B18" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>